<commit_message>
check point, navigate login page
</commit_message>
<xml_diff>
--- a/education api list(2).xlsx
+++ b/education api list(2).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github uploads\EK_tech_test_project\Project_testing_EK_tech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github uploads\Project_for_EK_TECH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A34891-9B22-4974-80FA-8931A7AAB948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EEC29E-E979-4B72-A752-D026086D234F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22128" yWindow="1224" windowWidth="21156" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>